<commit_message>
took out form action
</commit_message>
<xml_diff>
--- a/python_scripts/RSVP for Wedding.xlsx
+++ b/python_scripts/RSVP for Wedding.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invite" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="319">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -429,6 +429,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">조승</t>
     </r>
@@ -977,13 +978,44 @@
   <si>
     <t xml:space="preserve">song3</t>
   </si>
+  <si>
+    <t xml:space="preserve">Tue, 06 Aug 2024 14:27:14 GMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Joining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bohemian Rhapsody - Queen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagine - John Lennon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hey Jude - The Beatles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue, 06 Aug 2024 14:28:17 GMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carl Kotze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like a Rolling Stone - Bob Dylan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billie Jean - Michael Jackson</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1013,6 +1045,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1064,13 +1097,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1092,11 +1133,11 @@
   </sheetPr>
   <dimension ref="A1:F1022"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E100" activeCellId="0" sqref="E100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -1135,7 +1176,7 @@
       <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="b">
+      <c r="E2" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1157,7 +1198,7 @@
       <c r="D3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="b">
+      <c r="E3" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1179,7 +1220,7 @@
       <c r="D4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="0" t="b">
+      <c r="E4" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1201,7 +1242,7 @@
       <c r="D5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="0" t="b">
+      <c r="E5" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1223,7 +1264,7 @@
       <c r="D6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="b">
+      <c r="E6" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1245,7 +1286,7 @@
       <c r="D7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="0" t="b">
+      <c r="E7" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1267,7 +1308,7 @@
       <c r="D8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="0" t="b">
+      <c r="E8" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1289,7 +1330,7 @@
       <c r="D9" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="0" t="b">
+      <c r="E9" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1311,7 +1352,7 @@
       <c r="D10" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="0" t="b">
+      <c r="E10" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1333,7 +1374,7 @@
       <c r="D11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="0" t="b">
+      <c r="E11" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1355,7 +1396,7 @@
       <c r="D12" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="0" t="b">
+      <c r="E12" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1377,7 +1418,7 @@
       <c r="D13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="0" t="b">
+      <c r="E13" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1399,7 +1440,7 @@
       <c r="D14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="0" t="b">
+      <c r="E14" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1421,7 +1462,7 @@
       <c r="D15" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="0" t="b">
+      <c r="E15" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1443,7 +1484,7 @@
       <c r="D16" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="0" t="b">
+      <c r="E16" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1465,7 +1506,7 @@
       <c r="D17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="0" t="b">
+      <c r="E17" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1487,7 +1528,7 @@
       <c r="D18" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="0" t="b">
+      <c r="E18" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1509,7 +1550,7 @@
       <c r="D19" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="0" t="b">
+      <c r="E19" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1531,7 +1572,7 @@
       <c r="D20" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="0" t="b">
+      <c r="E20" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1553,7 +1594,7 @@
       <c r="D21" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="0" t="b">
+      <c r="E21" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1575,7 +1616,7 @@
       <c r="D22" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="0" t="b">
+      <c r="E22" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1597,7 +1638,7 @@
       <c r="D23" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="0" t="b">
+      <c r="E23" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1619,7 +1660,7 @@
       <c r="D24" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="0" t="b">
+      <c r="E24" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1641,7 +1682,7 @@
       <c r="D25" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="0" t="b">
+      <c r="E25" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1663,7 +1704,7 @@
       <c r="D26" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="0" t="b">
+      <c r="E26" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1685,7 +1726,7 @@
       <c r="D27" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="0" t="b">
+      <c r="E27" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1707,7 +1748,7 @@
       <c r="D28" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="0" t="b">
+      <c r="E28" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1729,7 +1770,7 @@
       <c r="D29" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="0" t="b">
+      <c r="E29" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1751,7 +1792,7 @@
       <c r="D30" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="0" t="b">
+      <c r="E30" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1773,7 +1814,7 @@
       <c r="D31" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="0" t="b">
+      <c r="E31" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1795,7 +1836,7 @@
       <c r="D32" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="0" t="b">
+      <c r="E32" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1817,7 +1858,7 @@
       <c r="D33" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="0" t="b">
+      <c r="E33" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1839,7 +1880,7 @@
       <c r="D34" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="0" t="b">
+      <c r="E34" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1861,7 +1902,7 @@
       <c r="D35" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="0" t="b">
+      <c r="E35" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1883,7 +1924,7 @@
       <c r="D36" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="0" t="b">
+      <c r="E36" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1905,7 +1946,7 @@
       <c r="D37" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="0" t="b">
+      <c r="E37" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1927,7 +1968,7 @@
       <c r="D38" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="0" t="b">
+      <c r="E38" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1949,7 +1990,7 @@
       <c r="D39" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="0" t="b">
+      <c r="E39" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1971,7 +2012,7 @@
       <c r="D40" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E40" s="0" t="b">
+      <c r="E40" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1993,7 +2034,7 @@
       <c r="D41" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="0" t="b">
+      <c r="E41" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2015,7 +2056,7 @@
       <c r="D42" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="0" t="b">
+      <c r="E42" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2037,7 +2078,7 @@
       <c r="D43" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="0" t="b">
+      <c r="E43" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2059,7 +2100,7 @@
       <c r="D44" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="E44" s="0" t="b">
+      <c r="E44" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2081,7 +2122,7 @@
       <c r="D45" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="E45" s="0" t="b">
+      <c r="E45" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2103,7 +2144,7 @@
       <c r="D46" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="0" t="b">
+      <c r="E46" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2125,7 +2166,7 @@
       <c r="D47" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="E47" s="0" t="b">
+      <c r="E47" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2147,7 +2188,7 @@
       <c r="D48" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="0" t="b">
+      <c r="E48" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2169,7 +2210,7 @@
       <c r="D49" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E49" s="0" t="b">
+      <c r="E49" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2191,7 +2232,7 @@
       <c r="D50" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="E50" s="0" t="b">
+      <c r="E50" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2213,7 +2254,7 @@
       <c r="D51" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="E51" s="0" t="b">
+      <c r="E51" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2235,7 +2276,7 @@
       <c r="D52" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="E52" s="0" t="b">
+      <c r="E52" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3225,7 +3266,7 @@
       <c r="D97" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="E97" s="0" t="b">
+      <c r="E97" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3247,7 +3288,7 @@
       <c r="D98" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="E98" s="0" t="b">
+      <c r="E98" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3269,7 +3310,7 @@
       <c r="D99" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="E99" s="0" t="b">
+      <c r="E99" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3291,7 +3332,7 @@
       <c r="D100" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="E100" s="0" t="b">
+      <c r="E100" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4238,13 +4279,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
@@ -4253,23 +4294,60 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>